<commit_message>
latest edit and modifications
</commit_message>
<xml_diff>
--- a/example_excel.xlsx
+++ b/example_excel.xlsx
@@ -936,7 +936,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K22"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1068,7 +1068,7 @@
         </is>
       </c>
       <c r="E3" t="n">
-        <v>190999295</v>
+        <v>191020929</v>
       </c>
       <c r="F3" t="n">
         <v>4908</v>
@@ -1115,7 +1115,7 @@
         </is>
       </c>
       <c r="E4" t="n">
-        <v>191023039</v>
+        <v>191020946</v>
       </c>
       <c r="F4" t="n">
         <v>490</v>
@@ -1162,7 +1162,7 @@
         </is>
       </c>
       <c r="E5" t="n">
-        <v>190998279</v>
+        <v>191020871</v>
       </c>
       <c r="F5" t="n">
         <v>134</v>
@@ -1209,7 +1209,7 @@
         </is>
       </c>
       <c r="E6" t="n">
-        <v>190994382</v>
+        <v>191020870</v>
       </c>
       <c r="F6" t="n">
         <v>37321</v>
@@ -1256,7 +1256,7 @@
         </is>
       </c>
       <c r="E7" t="n">
-        <v>190993929</v>
+        <v>191020925</v>
       </c>
       <c r="F7" t="n">
         <v>2993</v>
@@ -1342,7 +1342,7 @@
         </is>
       </c>
       <c r="E9" t="n">
-        <v>190994786</v>
+        <v>191023017</v>
       </c>
       <c r="F9" t="n">
         <v>32642</v>
@@ -1389,7 +1389,7 @@
         </is>
       </c>
       <c r="E10" t="n">
-        <v>190994725</v>
+        <v>191022896</v>
       </c>
       <c r="F10" t="n">
         <v>7925</v>
@@ -1432,7 +1432,7 @@
         </is>
       </c>
       <c r="E11" t="n">
-        <v>190994916</v>
+        <v>191022897</v>
       </c>
       <c r="F11" t="n">
         <v>321</v>
@@ -1454,503 +1454,6 @@
         </is>
       </c>
       <c r="K11" t="inlineStr">
-        <is>
-          <t>LAB_EXPRESS</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="n">
-        <v>45870</v>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>VSA</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>VSA</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>VSA2033PM</t>
-        </is>
-      </c>
-      <c r="E12" t="n">
-        <v>190994098</v>
-      </c>
-      <c r="F12" t="n">
-        <v>603</v>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>LOS GATOS DOG AND CAT HOSPITAL</t>
-        </is>
-      </c>
-      <c r="H12" t="n">
-        <v>1</v>
-      </c>
-      <c r="I12" t="n">
-        <v>10</v>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>updated</t>
-        </is>
-      </c>
-      <c r="K12" t="inlineStr">
-        <is>
-          <t>LAB_EXPRESS</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="n">
-        <v>45870</v>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>VSA</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>VSA</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>VSA2033PM</t>
-        </is>
-      </c>
-      <c r="E13" t="n">
-        <v>190994775</v>
-      </c>
-      <c r="F13" t="n">
-        <v>89954</v>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>ARK VETERINARY CARE</t>
-        </is>
-      </c>
-      <c r="H13" t="n">
-        <v>1</v>
-      </c>
-      <c r="I13" t="n">
-        <v>3</v>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>updated</t>
-        </is>
-      </c>
-      <c r="K13" t="inlineStr">
-        <is>
-          <t>LAB_EXPRESS</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="n">
-        <v>45870</v>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>VSA</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>VSA</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>VSA2037PM</t>
-        </is>
-      </c>
-      <c r="E14" t="n">
-        <v>190994472</v>
-      </c>
-      <c r="F14" t="n">
-        <v>1804</v>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>CASTRO VALLEY COMPANION ANIMAL HOSPITAL</t>
-        </is>
-      </c>
-      <c r="H14" t="n">
-        <v>0</v>
-      </c>
-      <c r="I14" t="n">
-        <v>7</v>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>updated</t>
-        </is>
-      </c>
-      <c r="K14" t="inlineStr">
-        <is>
-          <t>LAB_EXPRESS</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="2" t="n">
-        <v>45870</v>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>VSA</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>VSA</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>VSA2302PM</t>
-        </is>
-      </c>
-      <c r="E15" t="n">
-        <v>191001437</v>
-      </c>
-      <c r="F15" t="n">
-        <v>311</v>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>MARIN PET HOSPITAL  (SAN RAFAEL)</t>
-        </is>
-      </c>
-      <c r="H15" t="n">
-        <v>8</v>
-      </c>
-      <c r="I15" t="n">
-        <v>2</v>
-      </c>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="inlineStr">
-        <is>
-          <t>LAB_EXPRESS</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="n">
-        <v>45870</v>
-      </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>VSA</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>VSA</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>VSA2303PM</t>
-        </is>
-      </c>
-      <c r="E16" t="n">
-        <v>190994461</v>
-      </c>
-      <c r="F16" t="n">
-        <v>384</v>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>ABBEY  VETERINARY HOSPITAL</t>
-        </is>
-      </c>
-      <c r="H16" t="n">
-        <v>10</v>
-      </c>
-      <c r="I16" t="n">
-        <v>5</v>
-      </c>
-      <c r="J16" t="inlineStr"/>
-      <c r="K16" t="inlineStr">
-        <is>
-          <t>LAB_EXPRESS</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="2" t="n">
-        <v>45870</v>
-      </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>VSA</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>VSJ</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>VSJ1031AM</t>
-        </is>
-      </c>
-      <c r="E17" t="n">
-        <v>191014815</v>
-      </c>
-      <c r="F17" t="n">
-        <v>401</v>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>ALTA VIEW ANIMAL HOSPITAL</t>
-        </is>
-      </c>
-      <c r="H17" t="n">
-        <v>2</v>
-      </c>
-      <c r="I17" t="n">
-        <v>6</v>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>updated</t>
-        </is>
-      </c>
-      <c r="K17" t="inlineStr">
-        <is>
-          <t>LAB_EXPRESS</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="2" t="n">
-        <v>45871</v>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>VSA</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>VSA</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>VSA3023SA</t>
-        </is>
-      </c>
-      <c r="E18" t="n">
-        <v>190994662</v>
-      </c>
-      <c r="F18" t="n">
-        <v>7967</v>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>FAIRVIEW ANIMAL HOSPITAL</t>
-        </is>
-      </c>
-      <c r="H18" t="n">
-        <v>0</v>
-      </c>
-      <c r="I18" t="n">
-        <v>2</v>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>updated</t>
-        </is>
-      </c>
-      <c r="K18" t="inlineStr">
-        <is>
-          <t>LAB_EXPRESS</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="2" t="n">
-        <v>45871</v>
-      </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>VSA</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>VSA</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>VSA3030SA</t>
-        </is>
-      </c>
-      <c r="E19" t="n">
-        <v>191002734</v>
-      </c>
-      <c r="F19" t="n">
-        <v>30881</v>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>LENITY VET SPECIALISTS &amp; EMERGENCY CARE</t>
-        </is>
-      </c>
-      <c r="H19" t="n">
-        <v>8</v>
-      </c>
-      <c r="I19" t="n">
-        <v>3</v>
-      </c>
-      <c r="J19" t="inlineStr"/>
-      <c r="K19" t="inlineStr">
-        <is>
-          <t>LAB_EXPRESS</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="2" t="n">
-        <v>45871</v>
-      </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>VSA</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>VSA</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>VSA3030SA</t>
-        </is>
-      </c>
-      <c r="E20" t="n">
-        <v>190995197</v>
-      </c>
-      <c r="F20" t="n">
-        <v>754</v>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>NVA NORTH PENINSULA VET ER CLINIC 1</t>
-        </is>
-      </c>
-      <c r="H20" t="n">
-        <v>4</v>
-      </c>
-      <c r="I20" t="n">
-        <v>0</v>
-      </c>
-      <c r="J20" t="inlineStr"/>
-      <c r="K20" t="inlineStr">
-        <is>
-          <t>LAB_EXPRESS</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="2" t="n">
-        <v>45871</v>
-      </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>VSA</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>VSA</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>VSA3034SA</t>
-        </is>
-      </c>
-      <c r="E21" t="n">
-        <v>191017395</v>
-      </c>
-      <c r="F21" t="n">
-        <v>1869</v>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>EAST LAKE ANIMAL CLINIC</t>
-        </is>
-      </c>
-      <c r="H21" t="n">
-        <v>0</v>
-      </c>
-      <c r="I21" t="n">
-        <v>5</v>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>updated</t>
-        </is>
-      </c>
-      <c r="K21" t="inlineStr">
-        <is>
-          <t>LAB_EXPRESS</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="n">
-        <v>45871</v>
-      </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>VSA</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>VSA</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>VSA3043SA</t>
-        </is>
-      </c>
-      <c r="E22" t="n">
-        <v>190994731</v>
-      </c>
-      <c r="F22" t="n">
-        <v>1169</v>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>PINION ANIMAL HOSPITAL</t>
-        </is>
-      </c>
-      <c r="H22" t="n">
-        <v>3</v>
-      </c>
-      <c r="I22" t="n">
-        <v>2</v>
-      </c>
-      <c r="J22" t="inlineStr"/>
-      <c r="K22" t="inlineStr">
         <is>
           <t>LAB_EXPRESS</t>
         </is>

</xml_diff>